<commit_message>
add new test result
</commit_message>
<xml_diff>
--- a/results_process/align.xlsx
+++ b/results_process/align.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>split0001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -430,7 +430,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -501,6 +501,12 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>13322880</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
add new test results and update the record file and add a show figure scription
</commit_message>
<xml_diff>
--- a/results_process/align.xlsx
+++ b/results_process/align.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>split0001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -430,7 +430,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -505,6 +505,18 @@
         <v>13322880</v>
       </c>
       <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new test results
</commit_message>
<xml_diff>
--- a/results_process/align.xlsx
+++ b/results_process/align.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>split0001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -430,7 +430,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -524,6 +524,12 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>13335840</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
@@ -553,6 +559,12 @@
     <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>10</v>
+      </c>
+      <c r="B12">
+        <v>13258080</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7">

</xml_diff>